<commit_message>
add stuct pic in the dir
</commit_message>
<xml_diff>
--- a/struct.xlsx
+++ b/struct.xlsx
@@ -428,9 +428,9 @@
         <xdr:grpSpPr>
           <a:xfrm>
             <a:off x="8107680" y="2476500"/>
-            <a:ext cx="1889760" cy="739140"/>
+            <a:ext cx="1706880" cy="739140"/>
             <a:chOff x="-807720" y="4015740"/>
-            <a:chExt cx="1889760" cy="739140"/>
+            <a:chExt cx="1706880" cy="739140"/>
           </a:xfrm>
         </xdr:grpSpPr>
         <xdr:sp macro="" textlink="">
@@ -526,7 +526,7 @@
           <xdr:spPr>
             <a:xfrm>
               <a:off x="190500" y="4419600"/>
-              <a:ext cx="891540" cy="281940"/>
+              <a:ext cx="708660" cy="281940"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -901,7 +901,7 @@
             </xdr:nvSpPr>
             <xdr:spPr>
               <a:xfrm>
-                <a:off x="1988820" y="1668780"/>
+                <a:off x="1958340" y="1668780"/>
                 <a:ext cx="777240" cy="274320"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
@@ -3132,8 +3132,8 @@
             </xdr:nvSpPr>
             <xdr:spPr>
               <a:xfrm>
-                <a:off x="2026920" y="1539240"/>
-                <a:ext cx="777240" cy="365760"/>
+                <a:off x="1958340" y="1539240"/>
+                <a:ext cx="845820" cy="266700"/>
               </a:xfrm>
               <a:prstGeom prst="rect">
                 <a:avLst/>
@@ -3759,6 +3759,525 @@
     </xdr:cxnSp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>243839</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>68579</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Oval 20"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8122920" y="1851660"/>
+          <a:ext cx="45719" cy="45719"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>175259</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>144779</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="96" name="Oval 95"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5615940" y="1013460"/>
+          <a:ext cx="45719" cy="45719"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>45720</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>91439</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="97" name="Oval 96"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5532120" y="1348740"/>
+          <a:ext cx="45719" cy="45719"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="accent2"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>175260</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>179070</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="51" name="Straight Arrow Connector 50"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="16" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2796540" y="723900"/>
+          <a:ext cx="403860" cy="3810"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>426720</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="106" name="TextBox 105"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2628900" y="464820"/>
+          <a:ext cx="845820" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>rom_in</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>99060</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="107" name="Straight Arrow Connector 106"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="32" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5768340" y="792480"/>
+          <a:ext cx="426720" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="110" name="TextBox 109"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5646420" y="533400"/>
+          <a:ext cx="845820" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>ram_in</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>22860</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="111" name="Straight Arrow Connector 110"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="22" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7947660" y="3059430"/>
+          <a:ext cx="762000" cy="3810"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="25400">
+          <a:solidFill>
+            <a:schemeClr val="accent6"/>
+          </a:solidFill>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="112" name="TextBox 111"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7924800" y="2827020"/>
+          <a:ext cx="845820" cy="266700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" altLang="zh-CN" sz="1100"/>
+            <a:t>ram_out</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -4028,7 +4547,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+      <selection activeCell="P23" sqref="P23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>